<commit_message>
XLSX File accepted !
</commit_message>
<xml_diff>
--- a/csv_examples/example20chemicals.xlsx
+++ b/csv_examples/example20chemicals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Documents\GitHub\ChemicalSimilarityViewer\csv_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565F16F1-ADEA-4983-8D61-3421A1F83654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C157520-5D68-4CF6-88D0-6F8F16A4D02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -989,7 +989,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>